<commit_message>
Endurance Points, Fuel running now off LapData
</commit_message>
<xml_diff>
--- a/FuelConsumption.xlsx
+++ b/FuelConsumption.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melab2\Downloads\Aero_LapSim_11_1_14_(from_7-20)-2015-03-16\Aero LapSim 11_1_14 (from 7-20)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Journey\Documents\GitHub\LapSimCombined\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -348,257 +348,453 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A49"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <f>2.25*A1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <f t="shared" ref="B2:B48" si="0">2.25*A2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1.85098333333333E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>4.164712499999992E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1.9045055555555557E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>4.2851375000000002E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1.9039444444444444E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>4.2838750000000004E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2.0448277777777779E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>4.6008625000000004E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2.2960749999999999E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>5.1661687500000001E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2.4782833333333336E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>5.5761375000000007E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2.5436111111111111E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>5.7231249999999999E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2.5701944444444448E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>5.7829375000000008E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2.6519972222222199E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>5.9669937499999947E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2.8403333333333332E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>6.3907499999999997E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>3.0520277777777776E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>6.8670624999999999E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>3.2689166666666669E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>7.3550625000000005E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>3.4573888888888888E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>7.7791249999999996E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>3.6289166666666666E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>8.1650625000000004E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>3.7654166666666669E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>8.4721875000000006E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>3.8935000000000003E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>8.7603750000000008E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>4.0263333333333332E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>9.0592499999999996E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>4.1592222222222221E-3</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>9.3582500000000002E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>4.3083055555555557E-3</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>9.6936875000000009E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>4.4165000000000003E-3</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>9.9371250000000015E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>4.489666666666667E-3</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>1.0101750000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>4.5400000000000006E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>1.0215000000000002E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>4.5696666666666672E-3</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>1.0281750000000001E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>4.5668055555555557E-3</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>1.02753125E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>4.5398611111111108E-3</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>1.02146875E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>4.4973055555555556E-3</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>1.0118937499999999E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>4.4476111111111105E-3</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>1.0007124999999999E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>4.3783055555555554E-3</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>9.8511875000000006E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>4.3087500000000001E-3</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>9.6946875000000002E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>4.3311388888888887E-3</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>9.7450625000000003E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>4.3428611111111107E-3</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>9.7714374999999989E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>4.386277777777778E-3</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>9.8691250000000012E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>4.4377222222222222E-3</v>
+      </c>
+      <c r="B49">
+        <f>2.25*A49</f>
+        <v>9.9848750000000007E-3</v>
       </c>
     </row>
   </sheetData>
@@ -614,9 +810,9 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -636,7 +832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>250</v>
       </c>
@@ -648,7 +844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>500</v>
       </c>
@@ -660,7 +856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>750</v>
       </c>
@@ -672,7 +868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1000</v>
       </c>
@@ -684,7 +880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1250</v>
       </c>
@@ -696,7 +892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1500</v>
       </c>
@@ -708,7 +904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1750</v>
       </c>
@@ -720,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2000</v>
       </c>
@@ -732,7 +928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2250</v>
       </c>
@@ -744,7 +940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2500</v>
       </c>
@@ -756,7 +952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2750</v>
       </c>
@@ -768,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>3000</v>
       </c>
@@ -780,7 +976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>3250</v>
       </c>
@@ -792,7 +988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3500</v>
       </c>
@@ -804,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>3750</v>
       </c>
@@ -816,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>4000</v>
       </c>
@@ -828,7 +1024,7 @@
         <v>1.8509833333333334E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>4250</v>
       </c>
@@ -840,7 +1036,7 @@
         <v>1.9045055555555557E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>4500</v>
       </c>
@@ -852,7 +1048,7 @@
         <v>1.9039444444444444E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>4750</v>
       </c>
@@ -864,7 +1060,7 @@
         <v>2.0448277777777779E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>5000</v>
       </c>
@@ -876,7 +1072,7 @@
         <v>2.2960749999999999E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>5250</v>
       </c>
@@ -888,7 +1084,7 @@
         <v>2.4782833333333336E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>5500</v>
       </c>
@@ -900,7 +1096,7 @@
         <v>2.5436111111111111E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>5750</v>
       </c>
@@ -912,7 +1108,7 @@
         <v>2.5701944444444448E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>6000</v>
       </c>
@@ -924,7 +1120,7 @@
         <v>2.6519972222222225E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>6250</v>
       </c>
@@ -936,7 +1132,7 @@
         <v>2.8403333333333332E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>6500</v>
       </c>
@@ -948,7 +1144,7 @@
         <v>3.0520277777777776E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>6750</v>
       </c>
@@ -960,7 +1156,7 @@
         <v>3.2689166666666669E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>7000</v>
       </c>
@@ -972,7 +1168,7 @@
         <v>3.4573888888888888E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>7250</v>
       </c>
@@ -984,7 +1180,7 @@
         <v>3.6289166666666666E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>7500</v>
       </c>
@@ -996,7 +1192,7 @@
         <v>3.7654166666666669E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>7750</v>
       </c>
@@ -1008,7 +1204,7 @@
         <v>3.8935000000000003E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>8000</v>
       </c>
@@ -1020,7 +1216,7 @@
         <v>4.0263333333333332E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>8250</v>
       </c>
@@ -1032,7 +1228,7 @@
         <v>4.1592222222222221E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>8500</v>
       </c>
@@ -1044,7 +1240,7 @@
         <v>4.3083055555555557E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>8750</v>
       </c>
@@ -1056,7 +1252,7 @@
         <v>4.4165000000000003E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>9000</v>
       </c>
@@ -1068,7 +1264,7 @@
         <v>4.489666666666667E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>9250</v>
       </c>
@@ -1080,7 +1276,7 @@
         <v>4.5400000000000006E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>9500</v>
       </c>
@@ -1092,7 +1288,7 @@
         <v>4.5696666666666672E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>9750</v>
       </c>
@@ -1104,7 +1300,7 @@
         <v>4.5668055555555557E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>10000</v>
       </c>
@@ -1116,7 +1312,7 @@
         <v>4.5398611111111108E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>10250</v>
       </c>
@@ -1128,7 +1324,7 @@
         <v>4.4973055555555556E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>10500</v>
       </c>
@@ -1140,7 +1336,7 @@
         <v>4.4476111111111105E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>10750</v>
       </c>
@@ -1152,7 +1348,7 @@
         <v>4.3783055555555554E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>11000</v>
       </c>
@@ -1164,7 +1360,7 @@
         <v>4.3087500000000001E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>11250</v>
       </c>
@@ -1176,7 +1372,7 @@
         <v>4.3311388888888887E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>11500</v>
       </c>
@@ -1188,7 +1384,7 @@
         <v>4.3428611111111107E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>11750</v>
       </c>
@@ -1200,7 +1396,7 @@
         <v>4.386277777777778E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>12000</v>
       </c>

</xml_diff>

<commit_message>
Commit before investigating fix for RPM histogram
</commit_message>
<xml_diff>
--- a/FuelConsumption.xlsx
+++ b/FuelConsumption.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -83,6 +83,1606 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15712270341207349"/>
+          <c:y val="5.0925925925925923E-2"/>
+          <c:w val="0.76445975503062114"/>
+          <c:h val="0.79442913385826774"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Single Cylinder</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$1:$D$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2750</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3250</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3750</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4250</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4750</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5250</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5750</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6250</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6750</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7250</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7750</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8250</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8500</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8750</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9250</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9750</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10250</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>10500</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>10750</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>11250</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>11500</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>11750</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>12000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$1:$A$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.85098333333333E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.9045055555555557E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.9039444444444444E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.0448277777777779E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.2960749999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.4782833333333336E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.5436111111111111E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.5701944444444448E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.6519972222222199E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.8403333333333332E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.0520277777777776E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.2689166666666669E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.4573888888888888E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.6289166666666666E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.7654166666666669E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.8935000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.0263333333333332E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.1592222222222221E-3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.3083055555555557E-3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.4165000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.489666666666667E-3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.5400000000000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.5696666666666672E-3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.5668055555555557E-3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.5398611111111108E-3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.4973055555555556E-3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.4476111111111105E-3</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.3783055555555554E-3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.3087500000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.3311388888888887E-3</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.3428611111111107E-3</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.386277777777778E-3</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.4377222222222222E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Four Cylinder</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$1:$D$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2750</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3250</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3750</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4250</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4750</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5250</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5750</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6250</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6750</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7250</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7750</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8250</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8500</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8750</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9250</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9750</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10250</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>10500</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>10750</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>11250</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>11500</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>11750</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>12000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$B$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.164712499999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.2851375000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.2838750000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.6008625000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.1661687500000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.5761375000000007E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.7231249999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.7829375000000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.9669937499999947E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.3907499999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.8670624999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.3550625000000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.7791249999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8.1650625000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8.4721875000000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8.7603750000000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9.0592499999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9.3582500000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.6936875000000009E-3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.9371250000000015E-3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.0101750000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.0215000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.0281750000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.02753125E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.02146875E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.0118937499999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.0007124999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>9.8511875000000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9.6946875000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9.7450625000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>9.7714374999999989E-3</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>9.8691250000000012E-3</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9.9848750000000007E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="397080800"/>
+        <c:axId val="397085896"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="397080800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Engine</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Speed [RPM]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397085896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="397085896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Fuel</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Consumption at WOT [L/s]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397080800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19213801399825023"/>
+          <c:y val="9.3170749489647153E-2"/>
+          <c:w val="0.23286198600174979"/>
+          <c:h val="0.15625109361329836"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>53975</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>358775</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -348,15 +1948,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>0</v>
       </c>
@@ -364,8 +1964,11 @@
         <f>2.25*A1</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -373,8 +1976,11 @@
         <f t="shared" ref="B2:B48" si="0">2.25*A2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0</v>
       </c>
@@ -382,8 +1988,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0</v>
       </c>
@@ -391,8 +2000,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0</v>
       </c>
@@ -400,8 +2012,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0</v>
       </c>
@@ -409,8 +2024,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0</v>
       </c>
@@ -418,8 +2036,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D7">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0</v>
       </c>
@@ -427,8 +2048,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0</v>
       </c>
@@ -436,8 +2060,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0</v>
       </c>
@@ -445,8 +2072,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0</v>
       </c>
@@ -454,8 +2084,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D11">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0</v>
       </c>
@@ -463,8 +2096,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D12">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0</v>
       </c>
@@ -472,8 +2108,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D13">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0</v>
       </c>
@@ -481,8 +2120,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D14">
+        <v>3250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0</v>
       </c>
@@ -490,8 +2132,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D15">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0</v>
       </c>
@@ -499,8 +2144,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D16">
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1.85098333333333E-3</v>
       </c>
@@ -508,8 +2156,11 @@
         <f t="shared" si="0"/>
         <v>4.164712499999992E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D17">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1.9045055555555557E-3</v>
       </c>
@@ -517,8 +2168,11 @@
         <f t="shared" si="0"/>
         <v>4.2851375000000002E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D18">
+        <v>4250</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1.9039444444444444E-3</v>
       </c>
@@ -526,8 +2180,11 @@
         <f t="shared" si="0"/>
         <v>4.2838750000000004E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D19">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2.0448277777777779E-3</v>
       </c>
@@ -535,8 +2192,11 @@
         <f t="shared" si="0"/>
         <v>4.6008625000000004E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D20">
+        <v>4750</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2.2960749999999999E-3</v>
       </c>
@@ -544,8 +2204,11 @@
         <f t="shared" si="0"/>
         <v>5.1661687500000001E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D21">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2.4782833333333336E-3</v>
       </c>
@@ -553,8 +2216,11 @@
         <f t="shared" si="0"/>
         <v>5.5761375000000007E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D22">
+        <v>5250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2.5436111111111111E-3</v>
       </c>
@@ -562,8 +2228,11 @@
         <f t="shared" si="0"/>
         <v>5.7231249999999999E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D23">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2.5701944444444448E-3</v>
       </c>
@@ -571,8 +2240,11 @@
         <f t="shared" si="0"/>
         <v>5.7829375000000008E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D24">
+        <v>5750</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2.6519972222222199E-3</v>
       </c>
@@ -580,8 +2252,11 @@
         <f t="shared" si="0"/>
         <v>5.9669937499999947E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D25">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2.8403333333333332E-3</v>
       </c>
@@ -589,8 +2264,11 @@
         <f t="shared" si="0"/>
         <v>6.3907499999999997E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D26">
+        <v>6250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>3.0520277777777776E-3</v>
       </c>
@@ -598,8 +2276,11 @@
         <f t="shared" si="0"/>
         <v>6.8670624999999999E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D27">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>3.2689166666666669E-3</v>
       </c>
@@ -607,8 +2288,11 @@
         <f t="shared" si="0"/>
         <v>7.3550625000000005E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D28">
+        <v>6750</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>3.4573888888888888E-3</v>
       </c>
@@ -616,8 +2300,11 @@
         <f t="shared" si="0"/>
         <v>7.7791249999999996E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D29">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>3.6289166666666666E-3</v>
       </c>
@@ -625,8 +2312,11 @@
         <f t="shared" si="0"/>
         <v>8.1650625000000004E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D30">
+        <v>7250</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>3.7654166666666669E-3</v>
       </c>
@@ -634,8 +2324,11 @@
         <f t="shared" si="0"/>
         <v>8.4721875000000006E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D31">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>3.8935000000000003E-3</v>
       </c>
@@ -643,8 +2336,11 @@
         <f t="shared" si="0"/>
         <v>8.7603750000000008E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D32">
+        <v>7750</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>4.0263333333333332E-3</v>
       </c>
@@ -652,8 +2348,11 @@
         <f t="shared" si="0"/>
         <v>9.0592499999999996E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D33">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>4.1592222222222221E-3</v>
       </c>
@@ -661,8 +2360,11 @@
         <f t="shared" si="0"/>
         <v>9.3582500000000002E-3</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D34">
+        <v>8250</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>4.3083055555555557E-3</v>
       </c>
@@ -670,8 +2372,11 @@
         <f t="shared" si="0"/>
         <v>9.6936875000000009E-3</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D35">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>4.4165000000000003E-3</v>
       </c>
@@ -679,8 +2384,11 @@
         <f t="shared" si="0"/>
         <v>9.9371250000000015E-3</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D36">
+        <v>8750</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>4.489666666666667E-3</v>
       </c>
@@ -688,8 +2396,11 @@
         <f t="shared" si="0"/>
         <v>1.0101750000000001E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D37">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>4.5400000000000006E-3</v>
       </c>
@@ -697,8 +2408,11 @@
         <f t="shared" si="0"/>
         <v>1.0215000000000002E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D38">
+        <v>9250</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>4.5696666666666672E-3</v>
       </c>
@@ -706,8 +2420,11 @@
         <f t="shared" si="0"/>
         <v>1.0281750000000001E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D39">
+        <v>9500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>4.5668055555555557E-3</v>
       </c>
@@ -715,8 +2432,11 @@
         <f t="shared" si="0"/>
         <v>1.02753125E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D40">
+        <v>9750</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>4.5398611111111108E-3</v>
       </c>
@@ -724,8 +2444,11 @@
         <f t="shared" si="0"/>
         <v>1.02146875E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D41">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>4.4973055555555556E-3</v>
       </c>
@@ -733,8 +2456,11 @@
         <f t="shared" si="0"/>
         <v>1.0118937499999999E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D42">
+        <v>10250</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>4.4476111111111105E-3</v>
       </c>
@@ -742,8 +2468,11 @@
         <f t="shared" si="0"/>
         <v>1.0007124999999999E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D43">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>4.3783055555555554E-3</v>
       </c>
@@ -751,8 +2480,11 @@
         <f t="shared" si="0"/>
         <v>9.8511875000000006E-3</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D44">
+        <v>10750</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>4.3087500000000001E-3</v>
       </c>
@@ -760,8 +2492,11 @@
         <f t="shared" si="0"/>
         <v>9.6946875000000002E-3</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D45">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>4.3311388888888887E-3</v>
       </c>
@@ -769,8 +2504,11 @@
         <f t="shared" si="0"/>
         <v>9.7450625000000003E-3</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D46">
+        <v>11250</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>4.3428611111111107E-3</v>
       </c>
@@ -778,8 +2516,11 @@
         <f t="shared" si="0"/>
         <v>9.7714374999999989E-3</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D47">
+        <v>11500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>4.386277777777778E-3</v>
       </c>
@@ -787,8 +2528,11 @@
         <f t="shared" si="0"/>
         <v>9.8691250000000012E-3</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D48">
+        <v>11750</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>4.4377222222222222E-3</v>
       </c>
@@ -796,9 +2540,13 @@
         <f>2.25*A49</f>
         <v>9.9848750000000007E-3</v>
       </c>
+      <c r="D49">
+        <v>12000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>